<commit_message>
Finished se Zeitplan, Hans
Sorry if this is not your humor
</commit_message>
<xml_diff>
--- a/documentation/Zeitplan.xlsx
+++ b/documentation/Zeitplan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2438C719-53C2-4B28-8926-BAD28F1A9506}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FC20A6-B7B4-494A-86C9-29C090BA3DE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="490" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Aufwand SOLL</t>
   </si>
@@ -73,40 +73,7 @@
     <t>3. Realisierung</t>
   </si>
   <si>
-    <t>3.1 Installation Betriebsysteme</t>
-  </si>
-  <si>
-    <t>3.2 Voraussetzungen SCCM (Features)</t>
-  </si>
-  <si>
-    <t>3.3 Installation/Konfiguration MS SQL Server</t>
-  </si>
-  <si>
-    <t>3.4 Installation/Konfiguration SCCM</t>
-  </si>
-  <si>
-    <t>3.5 Installation/Konfiguration WDS</t>
-  </si>
-  <si>
-    <t>3.6 OS-Verteilung konfigurieren</t>
-  </si>
-  <si>
-    <t>3.7 MS-Office-Verteilung konfigurieren</t>
-  </si>
-  <si>
-    <t>3.8 OS verteilen</t>
-  </si>
-  <si>
-    <t>3.9 MS-Office verteilen</t>
-  </si>
-  <si>
-    <t>3.10 Testsystem inistalisieren</t>
-  </si>
-  <si>
     <t>3.11 Tests durchführen</t>
-  </si>
-  <si>
-    <t>3.12 Bericht abschliessen+Reserve</t>
   </si>
   <si>
     <t>Total Aufwand SOLL</t>
@@ -150,27 +117,12 @@
     </r>
   </si>
   <si>
-    <t>1.7 Aufgabe/Anforderungen verfeinern</t>
-  </si>
-  <si>
-    <t>1.8 Lösungsvarianten/Entscheidungsmatrix</t>
-  </si>
-  <si>
-    <t>1.5 Situationsanalyse (Projektziele)</t>
-  </si>
-  <si>
-    <t>1.6 Situationsanalyse (Anforderungen)</t>
-  </si>
-  <si>
     <t>2.1 Architekturdiagram</t>
   </si>
   <si>
     <t>2.2 Use-Case Diagramm</t>
   </si>
   <si>
-    <t>2.3. Mockup</t>
-  </si>
-  <si>
     <t>2.4 Testkonzept erstellen</t>
   </si>
   <si>
@@ -217,6 +169,45 @@
   </si>
   <si>
     <t>06.01.21</t>
+  </si>
+  <si>
+    <t>2.3 Mockup</t>
+  </si>
+  <si>
+    <t>3.1 Projektumgebung erstellen</t>
+  </si>
+  <si>
+    <t>3.4 Einzelspieler Modus</t>
+  </si>
+  <si>
+    <t>3.2 Login</t>
+  </si>
+  <si>
+    <t>3.3 Homescreen</t>
+  </si>
+  <si>
+    <t>3.5 Mehrspieler Modus</t>
+  </si>
+  <si>
+    <t>3.6 Mehrspieler Modus mit Link</t>
+  </si>
+  <si>
+    <t>3.7 Mehrspieler Modus mit unbekanntem Spieler</t>
+  </si>
+  <si>
+    <t>3.8 Vergangene Spiele</t>
+  </si>
+  <si>
+    <t>1.6 Aufgabe/Anforderungen verfeinern</t>
+  </si>
+  <si>
+    <t>1.5 Projektziele definieren</t>
+  </si>
+  <si>
+    <t>1.7 Lösungsvarianten/Entscheidungsmatrix</t>
+  </si>
+  <si>
+    <t>3.12 Bericht abschliessen/Debugging</t>
   </si>
 </sst>
 </file>
@@ -266,7 +257,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,6 +267,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -421,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -452,6 +455,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -495,6 +501,18 @@
     </xf>
     <xf numFmtId="167" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -776,168 +794,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:X61"/>
+  <dimension ref="C2:X55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V18" sqref="V18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AG21" sqref="AG21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="2.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.1796875" customWidth="1"/>
     <col min="2" max="2" width="3.453125" customWidth="1"/>
     <col min="3" max="3" width="40.81640625" customWidth="1"/>
-    <col min="4" max="4" width="5.54296875" customWidth="1"/>
-    <col min="5" max="5" width="6.1796875" customWidth="1"/>
-    <col min="6" max="6" width="4.7265625" customWidth="1"/>
+    <col min="4" max="4" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="24" width="2.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:24" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="I2" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="J2" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="L2" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="M2" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="N2" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="P2" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q2" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="R2" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="S2" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="T2" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="U2" s="28" t="s">
+      <c r="S2" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="U2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="V2" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="W2" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="X2" s="28" t="s">
-        <v>41</v>
+      <c r="V2" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="W2" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="X2" s="29" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="3:24" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="28"/>
-      <c r="V3" s="28"/>
-      <c r="W3" s="28"/>
-      <c r="X3" s="28"/>
+        <v>21</v>
+      </c>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="29"/>
+      <c r="V3" s="29"/>
+      <c r="W3" s="29"/>
+      <c r="X3" s="29"/>
     </row>
     <row r="4" spans="3:24" x14ac:dyDescent="0.35">
       <c r="C4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="28"/>
-      <c r="U4" s="28"/>
-      <c r="V4" s="28"/>
-      <c r="W4" s="28"/>
-      <c r="X4" s="28"/>
+        <v>18</v>
+      </c>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="27"/>
+      <c r="T4" s="29"/>
+      <c r="U4" s="29"/>
+      <c r="V4" s="29"/>
+      <c r="W4" s="29"/>
+      <c r="X4" s="29"/>
     </row>
     <row r="5" spans="3:24" x14ac:dyDescent="0.35">
       <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="27"/>
-      <c r="S5" s="27"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="29"/>
-      <c r="W5" s="29"/>
-      <c r="X5" s="29"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="30"/>
+      <c r="U5" s="30"/>
+      <c r="V5" s="30"/>
+      <c r="W5" s="30"/>
+      <c r="X5" s="30"/>
     </row>
     <row r="6" spans="3:24" x14ac:dyDescent="0.35">
       <c r="C6" s="1" t="s">
@@ -966,22 +984,20 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="18">
-        <f>SUM(G7:X7)</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="18">
-        <f>SUM(G8:X8)</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="18">
+      <c r="D7" s="19">
+        <v>3</v>
+      </c>
+      <c r="E7" s="19">
+        <v>3</v>
+      </c>
+      <c r="F7" s="19">
         <f>SUM($D$7:D7)-SUM($E$7:E7)</f>
         <v>0</v>
       </c>
-      <c r="G7" s="8"/>
+      <c r="G7" s="31"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -1001,11 +1017,11 @@
       <c r="X7" s="13"/>
     </row>
     <row r="8" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="20"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="9"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="34"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
@@ -1025,18 +1041,16 @@
       <c r="X8" s="14"/>
     </row>
     <row r="9" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="18">
-        <f>SUM(G9:X9)</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="18">
-        <f>SUM(G10:X10)</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="18">
+      <c r="D9" s="19">
+        <v>3</v>
+      </c>
+      <c r="E9" s="19">
+        <v>3</v>
+      </c>
+      <c r="F9" s="19">
         <f>SUM($D$7:D9)-SUM($E$7:E9)</f>
         <v>0</v>
       </c>
@@ -1044,7 +1058,7 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
+      <c r="K9" s="32"/>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
@@ -1060,15 +1074,15 @@
       <c r="X9" s="15"/>
     </row>
     <row r="10" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="20"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
+      <c r="K10" s="34"/>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
@@ -1084,22 +1098,20 @@
       <c r="X10" s="14"/>
     </row>
     <row r="11" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="21">
-        <f>SUM(G11:X11)</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="21">
-        <f>SUM(G12:X12)</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="21">
+      <c r="D11" s="22">
+        <v>1</v>
+      </c>
+      <c r="E11" s="22">
+        <v>1</v>
+      </c>
+      <c r="F11" s="22">
         <f>SUM($D$7:D11)-SUM($E$7:E11)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="10"/>
+      <c r="G11" s="32"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
@@ -1119,11 +1131,11 @@
       <c r="X11" s="15"/>
     </row>
     <row r="12" spans="3:24" ht="10" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="24"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="9"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="34"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
@@ -1143,27 +1155,23 @@
       <c r="X12" s="14"/>
     </row>
     <row r="13" spans="3:24" ht="10" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="21">
-        <f>SUM(G13:X13)</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="21">
-        <f>SUM(G14:X14)</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="21">
+      <c r="D13" s="22">
+        <v>1</v>
+      </c>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22">
         <f>SUM($D$7:D13)-SUM($E$7:E13)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
+      <c r="L13" s="32"/>
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -1178,10 +1186,10 @@
       <c r="X13" s="15"/>
     </row>
     <row r="14" spans="3:24" ht="10" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="20"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
@@ -1202,27 +1210,23 @@
       <c r="X14" s="14"/>
     </row>
     <row r="15" spans="3:24" ht="10" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="21">
-        <f>SUM(G15:X15)</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="21">
-        <f>SUM(G16:X16)</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="21">
+      <c r="C15" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="22">
+        <v>1</v>
+      </c>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22">
         <f>SUM($D$7:D15)-SUM($E$7:E15)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
+      <c r="L15" s="32"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
@@ -1237,10 +1241,10 @@
       <c r="X15" s="15"/>
     </row>
     <row r="16" spans="3:24" ht="10" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="20"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -1261,27 +1265,23 @@
       <c r="X16" s="14"/>
     </row>
     <row r="17" spans="3:24" ht="10" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="21">
-        <f>SUM(G17:X17)</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="21">
-        <f>SUM(G18:X18)</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="21">
+      <c r="C17" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="22">
+        <v>1</v>
+      </c>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22">
         <f>SUM($D$7:D17)-SUM($E$7:E17)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
+      <c r="L17" s="32"/>
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
@@ -1296,10 +1296,10 @@
       <c r="X17" s="13"/>
     </row>
     <row r="18" spans="3:24" ht="10" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="20"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -1320,20 +1320,16 @@
       <c r="X18" s="13"/>
     </row>
     <row r="19" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="18">
-        <f>SUM(G19:X19)</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="18">
-        <f>SUM(G20:X20)</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="18">
+      <c r="C19" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="19">
+        <v>2</v>
+      </c>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19">
         <f>SUM($D$7:D19)-SUM($E$7:E19)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
@@ -1341,7 +1337,7 @@
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
+      <c r="M19" s="32"/>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
       <c r="P19" s="10"/>
@@ -1355,77 +1351,75 @@
       <c r="X19" s="15"/>
     </row>
     <row r="20" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="20"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="9"/>
-      <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
-      <c r="X20" s="14"/>
-    </row>
-    <row r="21" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="18">
-        <f>SUM(G21:X21)</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="18">
-        <f>SUM(G22:X22)</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="18">
-        <f>SUM($D$7:D21)-SUM($E$7:E21)</f>
-        <v>0</v>
-      </c>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
-      <c r="S21" s="10"/>
-      <c r="T21" s="10"/>
-      <c r="U21" s="10"/>
-      <c r="V21" s="10"/>
-      <c r="W21" s="10"/>
-      <c r="X21" s="15"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="13"/>
+    </row>
+    <row r="21" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+      <c r="X21" s="12"/>
     </row>
     <row r="22" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="20"/>
-      <c r="D22" s="19"/>
+      <c r="C22" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="19">
+        <v>1</v>
+      </c>
       <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
+      <c r="F22" s="19">
+        <f>SUM($D$7:D22)-SUM($E$7:E22)</f>
+        <v>6</v>
+      </c>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="16"/>
       <c r="O22" s="8"/>
       <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
@@ -1437,72 +1431,66 @@
       <c r="W22" s="8"/>
       <c r="X22" s="13"/>
     </row>
-    <row r="23" spans="3:24" x14ac:dyDescent="0.35">
-      <c r="C23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="11"/>
-      <c r="S23" s="11"/>
-      <c r="T23" s="11"/>
-      <c r="U23" s="11"/>
-      <c r="V23" s="11"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="12"/>
+    <row r="23" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="21"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="14"/>
     </row>
     <row r="24" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="18">
-        <f>SUM(G24:X24)</f>
-        <v>0</v>
-      </c>
-      <c r="E24" s="18">
-        <f>SUM(G25:X25)</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="18">
+      <c r="C24" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="19">
+        <v>4</v>
+      </c>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19">
         <f>SUM($D$7:D24)-SUM($E$7:E24)</f>
-        <v>0</v>
-      </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="8"/>
-      <c r="T24" s="8"/>
-      <c r="U24" s="8"/>
-      <c r="V24" s="8"/>
-      <c r="W24" s="8"/>
-      <c r="X24" s="13"/>
+        <v>10</v>
+      </c>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="10"/>
+      <c r="W24" s="10"/>
+      <c r="X24" s="15"/>
     </row>
     <row r="25" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="20"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
@@ -1523,20 +1511,16 @@
       <c r="X25" s="14"/>
     </row>
     <row r="26" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C26" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="18">
-        <f>SUM(G26:X26)</f>
-        <v>0</v>
-      </c>
-      <c r="E26" s="18">
-        <f>SUM(G27:X27)</f>
-        <v>0</v>
-      </c>
-      <c r="F26" s="18">
+      <c r="C26" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="19">
+        <v>4</v>
+      </c>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19">
         <f>SUM($D$7:D26)-SUM($E$7:E26)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
@@ -1545,7 +1529,7 @@
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
+      <c r="N26" s="32"/>
       <c r="O26" s="10"/>
       <c r="P26" s="10"/>
       <c r="Q26" s="10"/>
@@ -1558,10 +1542,10 @@
       <c r="X26" s="15"/>
     </row>
     <row r="27" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C27" s="20"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
@@ -1582,20 +1566,16 @@
       <c r="X27" s="14"/>
     </row>
     <row r="28" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C28" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="18">
-        <f>SUM(G28:X28)</f>
-        <v>0</v>
-      </c>
-      <c r="E28" s="18">
-        <f>SUM(G29:X29)</f>
-        <v>0</v>
-      </c>
-      <c r="F28" s="18">
+      <c r="C28" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="19">
+        <v>4</v>
+      </c>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19">
         <f>SUM($D$7:D28)-SUM($E$7:E28)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
@@ -1605,7 +1585,7 @@
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
+      <c r="O28" s="32"/>
       <c r="P28" s="10"/>
       <c r="Q28" s="10"/>
       <c r="R28" s="10"/>
@@ -1617,69 +1597,67 @@
       <c r="X28" s="15"/>
     </row>
     <row r="29" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C29" s="20"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
-      <c r="U29" s="9"/>
-      <c r="V29" s="9"/>
-      <c r="W29" s="9"/>
-      <c r="X29" s="14"/>
-    </row>
-    <row r="30" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C30" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="18">
-        <f>SUM(G30:X30)</f>
-        <v>0</v>
-      </c>
-      <c r="E30" s="18">
-        <f>SUM(G31:X31)</f>
-        <v>0</v>
-      </c>
-      <c r="F30" s="18">
-        <f>SUM($D$7:D30)-SUM($E$7:E30)</f>
-        <v>0</v>
-      </c>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="10"/>
-      <c r="Q30" s="10"/>
-      <c r="R30" s="10"/>
-      <c r="S30" s="10"/>
-      <c r="T30" s="10"/>
-      <c r="U30" s="10"/>
-      <c r="V30" s="10"/>
-      <c r="W30" s="10"/>
-      <c r="X30" s="15"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="8"/>
+      <c r="T29" s="8"/>
+      <c r="U29" s="8"/>
+      <c r="V29" s="8"/>
+      <c r="W29" s="8"/>
+      <c r="X29" s="13"/>
+    </row>
+    <row r="30" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="11"/>
+      <c r="V30" s="11"/>
+      <c r="W30" s="11"/>
+      <c r="X30" s="12"/>
     </row>
     <row r="31" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C31" s="20"/>
-      <c r="D31" s="19"/>
+      <c r="C31" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="19">
+        <v>2</v>
+      </c>
       <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
+      <c r="F31" s="19">
+        <f>SUM($D$7:D31)-SUM($E$7:E31)</f>
+        <v>20</v>
+      </c>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
@@ -1689,7 +1667,7 @@
       <c r="M31" s="8"/>
       <c r="N31" s="8"/>
       <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
+      <c r="P31" s="31"/>
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
       <c r="S31" s="8"/>
@@ -1699,72 +1677,66 @@
       <c r="W31" s="8"/>
       <c r="X31" s="13"/>
     </row>
-    <row r="32" spans="3:24" x14ac:dyDescent="0.35">
-      <c r="C32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="11"/>
-      <c r="R32" s="11"/>
-      <c r="S32" s="11"/>
-      <c r="T32" s="11"/>
-      <c r="U32" s="11"/>
-      <c r="V32" s="11"/>
-      <c r="W32" s="11"/>
-      <c r="X32" s="12"/>
+    <row r="32" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="21"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
+      <c r="R32" s="9"/>
+      <c r="S32" s="9"/>
+      <c r="T32" s="9"/>
+      <c r="U32" s="9"/>
+      <c r="V32" s="9"/>
+      <c r="W32" s="9"/>
+      <c r="X32" s="14"/>
     </row>
     <row r="33" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C33" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="18">
-        <f>SUM(G33:X33)</f>
-        <v>0</v>
-      </c>
-      <c r="E33" s="18">
-        <f>SUM(G34:X34)</f>
-        <v>0</v>
-      </c>
-      <c r="F33" s="18">
+      <c r="C33" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="19">
+        <v>4</v>
+      </c>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19">
         <f>SUM($D$7:D33)-SUM($E$7:E33)</f>
-        <v>0</v>
-      </c>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
-      <c r="T33" s="8"/>
-      <c r="U33" s="8"/>
-      <c r="V33" s="8"/>
-      <c r="W33" s="8"/>
-      <c r="X33" s="13"/>
+        <v>24</v>
+      </c>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="32"/>
+      <c r="Q33" s="32"/>
+      <c r="R33" s="10"/>
+      <c r="S33" s="10"/>
+      <c r="T33" s="10"/>
+      <c r="U33" s="10"/>
+      <c r="V33" s="10"/>
+      <c r="W33" s="10"/>
+      <c r="X33" s="15"/>
     </row>
     <row r="34" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C34" s="20"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
       <c r="I34" s="9"/>
@@ -1785,20 +1757,16 @@
       <c r="X34" s="14"/>
     </row>
     <row r="35" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C35" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35" s="18">
-        <f>SUM(G35:X35)</f>
-        <v>0</v>
-      </c>
-      <c r="E35" s="18">
-        <f>SUM(G36:X36)</f>
-        <v>0</v>
-      </c>
-      <c r="F35" s="18">
+      <c r="C35" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="19">
+        <v>2</v>
+      </c>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19">
         <f>SUM($D$7:D35)-SUM($E$7:E35)</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
@@ -1810,7 +1778,7 @@
       <c r="N35" s="10"/>
       <c r="O35" s="10"/>
       <c r="P35" s="10"/>
-      <c r="Q35" s="10"/>
+      <c r="Q35" s="32"/>
       <c r="R35" s="10"/>
       <c r="S35" s="10"/>
       <c r="T35" s="10"/>
@@ -1820,10 +1788,10 @@
       <c r="X35" s="15"/>
     </row>
     <row r="36" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C36" s="20"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
       <c r="I36" s="9"/>
@@ -1844,20 +1812,16 @@
       <c r="X36" s="14"/>
     </row>
     <row r="37" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C37" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D37" s="18">
-        <f>SUM(G37:X37)</f>
-        <v>0</v>
-      </c>
-      <c r="E37" s="18">
-        <f>SUM(G38:X38)</f>
-        <v>0</v>
-      </c>
-      <c r="F37" s="18">
+      <c r="C37" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="19">
+        <v>8</v>
+      </c>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19">
         <f>SUM($D$7:D37)-SUM($E$7:E37)</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
@@ -1869,8 +1833,8 @@
       <c r="N37" s="10"/>
       <c r="O37" s="10"/>
       <c r="P37" s="10"/>
-      <c r="Q37" s="10"/>
-      <c r="R37" s="10"/>
+      <c r="Q37" s="32"/>
+      <c r="R37" s="32"/>
       <c r="S37" s="10"/>
       <c r="T37" s="10"/>
       <c r="U37" s="10"/>
@@ -1879,10 +1843,10 @@
       <c r="X37" s="15"/>
     </row>
     <row r="38" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C38" s="20"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
@@ -1903,20 +1867,16 @@
       <c r="X38" s="14"/>
     </row>
     <row r="39" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C39" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" s="18">
-        <f>SUM(G39:X39)</f>
-        <v>0</v>
-      </c>
-      <c r="E39" s="18">
-        <f>SUM(G40:X40)</f>
-        <v>0</v>
-      </c>
-      <c r="F39" s="18">
+      <c r="C39" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" s="19">
+        <v>16</v>
+      </c>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19">
         <f>SUM($D$7:D39)-SUM($E$7:E39)</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G39" s="10"/>
       <c r="H39" s="10"/>
@@ -1929,19 +1889,19 @@
       <c r="O39" s="10"/>
       <c r="P39" s="10"/>
       <c r="Q39" s="10"/>
-      <c r="R39" s="10"/>
-      <c r="S39" s="10"/>
-      <c r="T39" s="10"/>
+      <c r="R39" s="32"/>
+      <c r="S39" s="32"/>
+      <c r="T39" s="32"/>
       <c r="U39" s="10"/>
       <c r="V39" s="10"/>
       <c r="W39" s="10"/>
       <c r="X39" s="15"/>
     </row>
     <row r="40" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C40" s="20"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
       <c r="I40" s="9"/>
@@ -1962,20 +1922,16 @@
       <c r="X40" s="14"/>
     </row>
     <row r="41" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C41" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" s="18">
-        <f>SUM(G41:X41)</f>
-        <v>0</v>
-      </c>
-      <c r="E41" s="18">
-        <f>SUM(G42:X42)</f>
-        <v>0</v>
-      </c>
-      <c r="F41" s="18">
+      <c r="C41" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D41" s="19">
+        <v>4</v>
+      </c>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19">
         <f>SUM($D$7:D41)-SUM($E$7:E41)</f>
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="G41" s="10"/>
       <c r="H41" s="10"/>
@@ -1990,17 +1946,17 @@
       <c r="Q41" s="10"/>
       <c r="R41" s="10"/>
       <c r="S41" s="10"/>
-      <c r="T41" s="10"/>
+      <c r="T41" s="32"/>
       <c r="U41" s="10"/>
       <c r="V41" s="10"/>
       <c r="W41" s="10"/>
       <c r="X41" s="15"/>
     </row>
     <row r="42" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C42" s="20"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
@@ -2021,20 +1977,16 @@
       <c r="X42" s="14"/>
     </row>
     <row r="43" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C43" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D43" s="18">
-        <f>SUM(G43:X43)</f>
-        <v>0</v>
-      </c>
-      <c r="E43" s="18">
-        <f>SUM(G44:X44)</f>
-        <v>0</v>
-      </c>
-      <c r="F43" s="18">
+      <c r="C43" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" s="19">
+        <v>4</v>
+      </c>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19">
         <f>SUM($D$7:D43)-SUM($E$7:E43)</f>
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="G43" s="10"/>
       <c r="H43" s="10"/>
@@ -2050,16 +2002,16 @@
       <c r="R43" s="10"/>
       <c r="S43" s="10"/>
       <c r="T43" s="10"/>
-      <c r="U43" s="10"/>
+      <c r="U43" s="32"/>
       <c r="V43" s="10"/>
       <c r="W43" s="10"/>
       <c r="X43" s="15"/>
     </row>
     <row r="44" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C44" s="20"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
       <c r="G44" s="9"/>
       <c r="H44" s="9"/>
       <c r="I44" s="9"/>
@@ -2080,20 +2032,16 @@
       <c r="X44" s="14"/>
     </row>
     <row r="45" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C45" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D45" s="18">
-        <f>SUM(G45:X45)</f>
-        <v>0</v>
-      </c>
-      <c r="E45" s="18">
-        <f>SUM(G46:X46)</f>
-        <v>0</v>
-      </c>
-      <c r="F45" s="18">
+      <c r="C45" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="19">
+        <v>4</v>
+      </c>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19">
         <f>SUM($D$7:D45)-SUM($E$7:E45)</f>
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="G45" s="10"/>
       <c r="H45" s="10"/>
@@ -2110,15 +2058,15 @@
       <c r="S45" s="10"/>
       <c r="T45" s="10"/>
       <c r="U45" s="10"/>
-      <c r="V45" s="10"/>
+      <c r="V45" s="32"/>
       <c r="W45" s="10"/>
       <c r="X45" s="15"/>
     </row>
     <row r="46" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C46" s="20"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
       <c r="G46" s="9"/>
       <c r="H46" s="9"/>
       <c r="I46" s="9"/>
@@ -2139,20 +2087,16 @@
       <c r="X46" s="14"/>
     </row>
     <row r="47" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C47" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D47" s="18">
-        <f>SUM(G47:X47)</f>
-        <v>0</v>
-      </c>
-      <c r="E47" s="18">
-        <f>SUM(G48:X48)</f>
-        <v>0</v>
-      </c>
-      <c r="F47" s="18">
+      <c r="C47" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="19">
+        <v>2</v>
+      </c>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19">
         <f>SUM($D$7:D47)-SUM($E$7:E47)</f>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="G47" s="10"/>
       <c r="H47" s="10"/>
@@ -2170,14 +2114,14 @@
       <c r="T47" s="10"/>
       <c r="U47" s="10"/>
       <c r="V47" s="10"/>
-      <c r="W47" s="10"/>
+      <c r="W47" s="32"/>
       <c r="X47" s="15"/>
     </row>
     <row r="48" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C48" s="20"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
       <c r="G48" s="9"/>
       <c r="H48" s="9"/>
       <c r="I48" s="9"/>
@@ -2198,20 +2142,16 @@
       <c r="X48" s="14"/>
     </row>
     <row r="49" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C49" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D49" s="18">
-        <f>SUM(G49:X49)</f>
-        <v>0</v>
-      </c>
-      <c r="E49" s="18">
-        <f>SUM(G50:X50)</f>
-        <v>0</v>
-      </c>
-      <c r="F49" s="18">
+      <c r="C49" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="19">
+        <v>8</v>
+      </c>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19">
         <f>SUM($D$7:D49)-SUM($E$7:E49)</f>
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
@@ -2229,268 +2169,91 @@
       <c r="T49" s="10"/>
       <c r="U49" s="10"/>
       <c r="V49" s="10"/>
-      <c r="W49" s="10"/>
-      <c r="X49" s="15"/>
+      <c r="W49" s="32"/>
+      <c r="X49" s="33"/>
     </row>
     <row r="50" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C50" s="20"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="9"/>
-      <c r="K50" s="9"/>
-      <c r="L50" s="9"/>
-      <c r="M50" s="9"/>
-      <c r="N50" s="9"/>
-      <c r="O50" s="9"/>
-      <c r="P50" s="9"/>
-      <c r="Q50" s="9"/>
-      <c r="R50" s="9"/>
-      <c r="S50" s="9"/>
-      <c r="T50" s="9"/>
-      <c r="U50" s="9"/>
-      <c r="V50" s="9"/>
-      <c r="W50" s="9"/>
-      <c r="X50" s="14"/>
-    </row>
-    <row r="51" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C51" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="D51" s="18">
-        <f>SUM(G51:X51)</f>
-        <v>0</v>
-      </c>
-      <c r="E51" s="18">
-        <f>SUM(G52:X52)</f>
-        <v>0</v>
-      </c>
-      <c r="F51" s="18">
-        <f>SUM($D$7:D51)-SUM($E$7:E51)</f>
-        <v>0</v>
-      </c>
-      <c r="G51" s="10"/>
-      <c r="H51" s="10"/>
-      <c r="I51" s="10"/>
-      <c r="J51" s="10"/>
-      <c r="K51" s="10"/>
-      <c r="L51" s="10"/>
-      <c r="M51" s="10"/>
-      <c r="N51" s="10"/>
-      <c r="O51" s="10"/>
-      <c r="P51" s="10"/>
-      <c r="Q51" s="10"/>
-      <c r="R51" s="10"/>
-      <c r="S51" s="10"/>
-      <c r="T51" s="10"/>
-      <c r="U51" s="10"/>
-      <c r="V51" s="10"/>
-      <c r="W51" s="10"/>
-      <c r="X51" s="15"/>
-    </row>
-    <row r="52" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C52" s="20"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="9"/>
-      <c r="J52" s="9"/>
-      <c r="K52" s="9"/>
-      <c r="L52" s="9"/>
-      <c r="M52" s="9"/>
-      <c r="N52" s="9"/>
-      <c r="O52" s="9"/>
-      <c r="P52" s="9"/>
-      <c r="Q52" s="9"/>
-      <c r="R52" s="9"/>
-      <c r="S52" s="9"/>
-      <c r="T52" s="9"/>
-      <c r="U52" s="9"/>
-      <c r="V52" s="9"/>
-      <c r="W52" s="9"/>
-      <c r="X52" s="14"/>
-    </row>
-    <row r="53" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C53" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D53" s="18">
-        <f>SUM(G53:X53)</f>
-        <v>0</v>
-      </c>
-      <c r="E53" s="18">
-        <f>SUM(G54:X54)</f>
-        <v>0</v>
-      </c>
-      <c r="F53" s="18">
-        <f>SUM($D$7:D53)-SUM($E$7:E53)</f>
-        <v>0</v>
-      </c>
-      <c r="G53" s="10"/>
-      <c r="H53" s="10"/>
-      <c r="I53" s="10"/>
-      <c r="J53" s="10"/>
-      <c r="K53" s="10"/>
-      <c r="L53" s="10"/>
-      <c r="M53" s="10"/>
-      <c r="N53" s="10"/>
-      <c r="O53" s="10"/>
-      <c r="P53" s="10"/>
-      <c r="Q53" s="10"/>
-      <c r="R53" s="10"/>
-      <c r="S53" s="10"/>
-      <c r="T53" s="10"/>
-      <c r="U53" s="10"/>
-      <c r="V53" s="10"/>
-      <c r="W53" s="10"/>
-      <c r="X53" s="15"/>
-    </row>
-    <row r="54" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C54" s="20"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
-      <c r="J54" s="9"/>
-      <c r="K54" s="9"/>
-      <c r="L54" s="9"/>
-      <c r="M54" s="9"/>
-      <c r="N54" s="9"/>
-      <c r="O54" s="9"/>
-      <c r="P54" s="9"/>
-      <c r="Q54" s="9"/>
-      <c r="R54" s="9"/>
-      <c r="S54" s="9"/>
-      <c r="T54" s="9"/>
-      <c r="U54" s="9"/>
-      <c r="V54" s="9"/>
-      <c r="W54" s="9"/>
-      <c r="X54" s="14"/>
-    </row>
-    <row r="55" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C55" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D55" s="18">
-        <f>SUM(G55:X55)</f>
-        <v>0</v>
-      </c>
-      <c r="E55" s="18">
-        <f>SUM(G56:X56)</f>
-        <v>0</v>
-      </c>
-      <c r="F55" s="18">
-        <f>SUM($D$7:D55)-SUM($E$7:E55)</f>
-        <v>0</v>
-      </c>
-      <c r="G55" s="10"/>
-      <c r="H55" s="10"/>
-      <c r="I55" s="10"/>
-      <c r="J55" s="10"/>
-      <c r="K55" s="10"/>
-      <c r="L55" s="10"/>
-      <c r="M55" s="10"/>
-      <c r="N55" s="10"/>
-      <c r="O55" s="10"/>
-      <c r="P55" s="10"/>
-      <c r="Q55" s="10"/>
-      <c r="R55" s="10"/>
-      <c r="S55" s="10"/>
-      <c r="T55" s="10"/>
-      <c r="U55" s="10"/>
-      <c r="V55" s="10"/>
-      <c r="W55" s="10"/>
-      <c r="X55" s="15"/>
-    </row>
-    <row r="56" spans="3:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C56" s="20"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="19"/>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="8"/>
-      <c r="K56" s="8"/>
-      <c r="L56" s="8"/>
-      <c r="M56" s="8"/>
-      <c r="N56" s="8"/>
-      <c r="O56" s="8"/>
-      <c r="P56" s="8"/>
-      <c r="Q56" s="8"/>
-      <c r="R56" s="8"/>
-      <c r="S56" s="8"/>
-      <c r="T56" s="8"/>
-      <c r="U56" s="8"/>
-      <c r="V56" s="8"/>
-      <c r="W56" s="8"/>
-      <c r="X56" s="13"/>
-    </row>
-    <row r="57" spans="3:24" x14ac:dyDescent="0.35">
-      <c r="C57" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
-      <c r="K57" s="2"/>
-      <c r="L57" s="2"/>
-      <c r="M57" s="2"/>
-      <c r="N57" s="2"/>
-      <c r="O57" s="2"/>
-      <c r="P57" s="2"/>
-      <c r="Q57" s="2"/>
-      <c r="R57" s="2"/>
-      <c r="S57" s="2"/>
-      <c r="T57" s="2"/>
-      <c r="U57" s="2"/>
-      <c r="V57" s="2"/>
-      <c r="W57" s="2"/>
-      <c r="X57" s="3"/>
-    </row>
-    <row r="59" spans="3:24" x14ac:dyDescent="0.35">
-      <c r="C59" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D59" s="7">
-        <f>SUM(D7:D56)</f>
-        <v>0</v>
-      </c>
-      <c r="E59" s="7"/>
-    </row>
-    <row r="60" spans="3:24" x14ac:dyDescent="0.35">
-      <c r="C60" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D60" s="6"/>
-      <c r="E60" s="7">
-        <f>SUM(E7:E56)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="3:24" x14ac:dyDescent="0.35">
-      <c r="C61" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D61" s="16">
-        <f>D59-E60</f>
-        <v>0</v>
-      </c>
-      <c r="E61" s="17"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="8"/>
+      <c r="L50" s="8"/>
+      <c r="M50" s="8"/>
+      <c r="N50" s="8"/>
+      <c r="O50" s="8"/>
+      <c r="P50" s="8"/>
+      <c r="Q50" s="8"/>
+      <c r="R50" s="8"/>
+      <c r="S50" s="8"/>
+      <c r="T50" s="8"/>
+      <c r="U50" s="8"/>
+      <c r="V50" s="8"/>
+      <c r="W50" s="8"/>
+      <c r="X50" s="13"/>
+    </row>
+    <row r="51" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C51" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2"/>
+      <c r="R51" s="2"/>
+      <c r="S51" s="2"/>
+      <c r="T51" s="2"/>
+      <c r="U51" s="2"/>
+      <c r="V51" s="2"/>
+      <c r="W51" s="2"/>
+      <c r="X51" s="3"/>
+    </row>
+    <row r="53" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C53" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="7">
+        <f>SUM(D7:D50)</f>
+        <v>79</v>
+      </c>
+      <c r="E53" s="7"/>
+    </row>
+    <row r="54" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C54" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D54" s="6"/>
+      <c r="E54" s="7">
+        <f>SUM(E7:E50)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C55" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="17">
+        <f>D53-E54</f>
+        <v>72</v>
+      </c>
+      <c r="E55" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="118">
+  <mergeCells count="106">
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
@@ -2502,7 +2265,6 @@
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
@@ -2513,78 +2275,67 @@
     <mergeCell ref="E17:E18"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C22:C23"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="E24:E25"/>
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="D26:D27"/>
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="F26:F27"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="C28:C29"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="F28:F29"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C47:C48"/>
     <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="C31:C32"/>
     <mergeCell ref="C33:C34"/>
     <mergeCell ref="C35:C36"/>
     <mergeCell ref="C37:C38"/>
     <mergeCell ref="C39:C40"/>
     <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
     <mergeCell ref="D37:D38"/>
     <mergeCell ref="E37:E38"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
     <mergeCell ref="D33:D34"/>
     <mergeCell ref="E33:E34"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
     <mergeCell ref="D45:D46"/>
     <mergeCell ref="E45:E46"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="D55:E55"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
     <mergeCell ref="F49:F50"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="F19:F20"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="D13:D14"/>

</xml_diff>